<commit_message>
Fix template downloads (generate template on the fly instead of serving a static file)
</commit_message>
<xml_diff>
--- a/experiments/xls/measurements_input.xlsx
+++ b/experiments/xls/measurements_input.xlsx
@@ -19,64 +19,64 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>fad84d2e-6351-47c8-815f-34e05df97642</t>
-  </si>
-  <si>
-    <t>f20ee2af-954f-4df2-82d8-16538b51153b</t>
-  </si>
-  <si>
-    <t>b2f8a771-0814-47b6-ad6b-a267c5881d20</t>
-  </si>
-  <si>
-    <t>c5627ec7-5290-4d63-bf1a-16435df4df27</t>
-  </si>
-  <si>
-    <t>0a064c75-e6da-46c5-806d-ed816cdd5989</t>
-  </si>
-  <si>
-    <t>612ec7a1-78dd-4db5-9504-50d69a1c8bac</t>
-  </si>
-  <si>
-    <t>c6509624-c0a1-4e88-82bf-d229aca2894e</t>
-  </si>
-  <si>
-    <t>85558a0b-b057-4e6b-8895-60fddd661d16</t>
-  </si>
-  <si>
-    <t>7f2697c9-d64e-4871-9f9e-337966ed4f45</t>
-  </si>
-  <si>
-    <t>458d7ca3-af50-4f9b-a5e2-87c2d5d37f96</t>
-  </si>
-  <si>
-    <t>d7f6f969-ebc6-467e-a56f-0113388a0897</t>
-  </si>
-  <si>
-    <t>f5329457-1db2-45ff-899f-b1f5b342c69f</t>
-  </si>
-  <si>
-    <t>dbfc57ef-ea13-493f-a169-12be4b8f0c68</t>
-  </si>
-  <si>
-    <t>7bf5ea72-3be5-4272-9def-c691430cc7ae</t>
-  </si>
-  <si>
-    <t>9a92360c-d991-42c5-bb77-79e8af10fc4f</t>
-  </si>
-  <si>
-    <t>c01445ac-a175-41ae-a324-0b859283bb77</t>
-  </si>
-  <si>
-    <t>72a2894c-ef20-431a-b341-9aef27456520</t>
-  </si>
-  <si>
-    <t>0dc8335b-066b-4a24-83bb-4bac135531aa</t>
-  </si>
-  <si>
-    <t>26c4646b-76ae-44bd-ac4f-38d28cc0c050</t>
-  </si>
-  <si>
-    <t>f344c7a7-f129-49ae-8f15-845419d7e936</t>
+    <t>1672e944-65e7-4e52-ba8c-17d2a5f7b348</t>
+  </si>
+  <si>
+    <t>10a11f2c-62ff-498e-b2ed-22a56f03fa05</t>
+  </si>
+  <si>
+    <t>e32069c9-901c-415a-8287-80d38e02cf86</t>
+  </si>
+  <si>
+    <t>7e55d992-14a1-4677-b1b2-51746d9043f3</t>
+  </si>
+  <si>
+    <t>2b4332a6-1a8a-4189-b14c-6cd8deda2b9d</t>
+  </si>
+  <si>
+    <t>5f997230-b51c-425e-9e18-0b2694b6663b</t>
+  </si>
+  <si>
+    <t>e6a70ac8-faf5-4f2d-8fd1-8836867f45a7</t>
+  </si>
+  <si>
+    <t>38e11126-1915-4965-9907-4daefcc9e279</t>
+  </si>
+  <si>
+    <t>66c48cfa-b3fb-46b2-83d8-94026a408ab7</t>
+  </si>
+  <si>
+    <t>ca8b67d2-4f44-47de-ae8a-42c5d546e0f9</t>
+  </si>
+  <si>
+    <t>5309928e-ada4-4446-8a0b-36905ce059d8</t>
+  </si>
+  <si>
+    <t>3d277d4a-ece3-4ab1-972e-040f8c7d28fe</t>
+  </si>
+  <si>
+    <t>b1531088-2f2a-4303-8541-f51f6eb0b10b</t>
+  </si>
+  <si>
+    <t>ab4e3112-df70-4e79-92b0-1cb588f5047f</t>
+  </si>
+  <si>
+    <t>5bde3542-13e7-4f5d-ba69-92e1b852b13f</t>
+  </si>
+  <si>
+    <t>7baaa21f-01a5-4a1d-a56d-4a619be80766</t>
+  </si>
+  <si>
+    <t>46efc080-c040-42f7-87be-d120ce5090c4</t>
+  </si>
+  <si>
+    <t>0df1abb7-4e8b-4606-85d3-37325621383b</t>
+  </si>
+  <si>
+    <t>e53d951e-cb2a-4be3-95d4-372fc377f278</t>
+  </si>
+  <si>
+    <t>474cc043-54d4-48ca-975e-7bce678492eb</t>
   </si>
   <si>
     <t>Mode</t>
@@ -770,45 +770,39 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="14">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mode" prompt="Choose mode" sqref="B2:B101">
       <formula1>"Ignore,Create or update,Delete"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Researcher" prompt="Choose researcher" sqref="C2:C101">
-      <formula1>"A_K,M_W"</formula1>
+      <formula1>"A_K,M_W,KR"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Project" prompt="Choose project" sqref="D2:D101">
-      <formula1>"ML_HEA,KB_CAH"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Slide" prompt="Choose slide" sqref="E2:E101">
-      <formula1>"S000000725,S000000724,S000000726,S000000729"</formula1>
+      <formula1>"ML_HEA,KB_CAH,TM_RCC"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G101">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H101">
-      <formula1>"S000000725,S000000724,S000000726,S000000729"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Technology" prompt="Choose technology" sqref="I2:I101">
-      <formula1>"RNAscope 4-plex,RNAscope 8-plex"</formula1>
+      <formula1>"RNAscope 4-plex,RNAscope 8-plex,RNAscope 3-plex + IHC"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J101">
       <formula1>10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Channel-target pair" prompt="Choose channel-target pair" sqref="K2:K101">
-      <formula1>"Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; POLR2A,Atto 425 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; MYH11"</formula1>
+      <formula1>"Atto 425 -&gt; MYH11,Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; POLR2A,DAPI -&gt; Nucleus,Opal 520 -&gt; PECAM1 (IHC),Opal 570 -&gt; CA9,Opal 650 -&gt; TPSB2,Atto 425 -&gt; CD68,Opal 570 -&gt; CMET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Channel-target pair" prompt="Choose channel-target pair" sqref="L2:L101">
-      <formula1>"Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; POLR2A,Atto 425 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; MYH11"</formula1>
+      <formula1>"Atto 425 -&gt; MYH11,Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; POLR2A,DAPI -&gt; Nucleus,Opal 520 -&gt; PECAM1 (IHC),Opal 570 -&gt; CA9,Opal 650 -&gt; TPSB2,Atto 425 -&gt; CD68,Opal 570 -&gt; CMET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Channel-target pair" prompt="Choose channel-target pair" sqref="M2:M101">
-      <formula1>"Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; POLR2A,Atto 425 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; MYH11"</formula1>
+      <formula1>"Atto 425 -&gt; MYH11,Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; POLR2A,DAPI -&gt; Nucleus,Opal 520 -&gt; PECAM1 (IHC),Opal 570 -&gt; CA9,Opal 650 -&gt; TPSB2,Atto 425 -&gt; CD68,Opal 570 -&gt; CMET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Channel-target pair" prompt="Choose channel-target pair" sqref="N2:N101">
-      <formula1>"Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; POLR2A,Atto 425 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; MYH11"</formula1>
+      <formula1>"Atto 425 -&gt; MYH11,Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; POLR2A,DAPI -&gt; Nucleus,Opal 520 -&gt; PECAM1 (IHC),Opal 570 -&gt; CA9,Opal 650 -&gt; TPSB2,Atto 425 -&gt; CD68,Opal 570 -&gt; CMET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Channel-target pair" prompt="Choose channel-target pair" sqref="O2:O101">
-      <formula1>"Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; POLR2A,Atto 425 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; MYH11"</formula1>
+      <formula1>"Atto 425 -&gt; MYH11,Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; POLR2A,DAPI -&gt; Nucleus,Opal 520 -&gt; PECAM1 (IHC),Opal 570 -&gt; CA9,Opal 650 -&gt; TPSB2,Atto 425 -&gt; CD68,Opal 570 -&gt; CMET"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Team directory" prompt="Choose team directory" sqref="Z2:Z101">
       <formula1>"t283_imaging,t876_imaging"</formula1>

</xml_diff>

<commit_message>
Add uuids generation endpoint
</commit_message>
<xml_diff>
--- a/experiments/xls/measurements_input.xlsx
+++ b/experiments/xls/measurements_input.xlsx
@@ -19,64 +19,64 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>1672e944-65e7-4e52-ba8c-17d2a5f7b348</t>
-  </si>
-  <si>
-    <t>10a11f2c-62ff-498e-b2ed-22a56f03fa05</t>
-  </si>
-  <si>
-    <t>e32069c9-901c-415a-8287-80d38e02cf86</t>
-  </si>
-  <si>
-    <t>7e55d992-14a1-4677-b1b2-51746d9043f3</t>
-  </si>
-  <si>
-    <t>2b4332a6-1a8a-4189-b14c-6cd8deda2b9d</t>
-  </si>
-  <si>
-    <t>5f997230-b51c-425e-9e18-0b2694b6663b</t>
-  </si>
-  <si>
-    <t>e6a70ac8-faf5-4f2d-8fd1-8836867f45a7</t>
-  </si>
-  <si>
-    <t>38e11126-1915-4965-9907-4daefcc9e279</t>
-  </si>
-  <si>
-    <t>66c48cfa-b3fb-46b2-83d8-94026a408ab7</t>
-  </si>
-  <si>
-    <t>ca8b67d2-4f44-47de-ae8a-42c5d546e0f9</t>
-  </si>
-  <si>
-    <t>5309928e-ada4-4446-8a0b-36905ce059d8</t>
-  </si>
-  <si>
-    <t>3d277d4a-ece3-4ab1-972e-040f8c7d28fe</t>
-  </si>
-  <si>
-    <t>b1531088-2f2a-4303-8541-f51f6eb0b10b</t>
-  </si>
-  <si>
-    <t>ab4e3112-df70-4e79-92b0-1cb588f5047f</t>
-  </si>
-  <si>
-    <t>5bde3542-13e7-4f5d-ba69-92e1b852b13f</t>
-  </si>
-  <si>
-    <t>7baaa21f-01a5-4a1d-a56d-4a619be80766</t>
-  </si>
-  <si>
-    <t>46efc080-c040-42f7-87be-d120ce5090c4</t>
-  </si>
-  <si>
-    <t>0df1abb7-4e8b-4606-85d3-37325621383b</t>
-  </si>
-  <si>
-    <t>e53d951e-cb2a-4be3-95d4-372fc377f278</t>
-  </si>
-  <si>
-    <t>474cc043-54d4-48ca-975e-7bce678492eb</t>
+    <t>4eaf7e16-598b-4e38-b01a-6f5d384ab235</t>
+  </si>
+  <si>
+    <t>f1e9d607-82b9-4c68-9a6b-5c591a9ded1f</t>
+  </si>
+  <si>
+    <t>fe96bab7-4a88-45a2-b017-dbca6b681a5a</t>
+  </si>
+  <si>
+    <t>877735e8-2407-45da-a3dc-527c19890f5f</t>
+  </si>
+  <si>
+    <t>61a7abc4-b9d4-4a7c-8287-1316bd955f07</t>
+  </si>
+  <si>
+    <t>0ecb761b-0d34-440c-8eee-8d9da3c4a923</t>
+  </si>
+  <si>
+    <t>88ce8b93-cad3-422c-b7f5-df423d83b939</t>
+  </si>
+  <si>
+    <t>8fc74982-3a71-4982-9cb5-af4b9017bd91</t>
+  </si>
+  <si>
+    <t>077adec4-8c75-4682-9168-6d3123921f91</t>
+  </si>
+  <si>
+    <t>9d582f70-b6ef-43e1-84f5-0f3c89933604</t>
+  </si>
+  <si>
+    <t>54ad7c88-dece-4a6b-9423-d1e45b87c01a</t>
+  </si>
+  <si>
+    <t>b06bd5d7-f6bd-4b6a-a73f-6a2afc623ae3</t>
+  </si>
+  <si>
+    <t>8a2b27c8-8587-45d2-bd83-92869b8d9cdd</t>
+  </si>
+  <si>
+    <t>da12c9fc-b68b-47fe-928b-8b01e2a9fea1</t>
+  </si>
+  <si>
+    <t>fbf29566-fd64-48d1-bf75-4dc4fce36120</t>
+  </si>
+  <si>
+    <t>62817df8-3580-45a2-8462-af545d87e573</t>
+  </si>
+  <si>
+    <t>79555e3a-e711-4720-8345-d99a3b126e2a</t>
+  </si>
+  <si>
+    <t>c13aa51c-02f4-435b-9180-d9d8a22d1161</t>
+  </si>
+  <si>
+    <t>e87e5057-3875-4a21-acfd-2c993173809b</t>
+  </si>
+  <si>
+    <t>ac3c581a-17ff-4162-bad2-cd2db03445c4</t>
   </si>
   <si>
     <t>Mode</t>

</xml_diff>

<commit_message>
Add optional and required columns
</commit_message>
<xml_diff>
--- a/experiments/xls/measurements_input.xlsx
+++ b/experiments/xls/measurements_input.xlsx
@@ -19,64 +19,64 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>4eaf7e16-598b-4e38-b01a-6f5d384ab235</t>
-  </si>
-  <si>
-    <t>f1e9d607-82b9-4c68-9a6b-5c591a9ded1f</t>
-  </si>
-  <si>
-    <t>fe96bab7-4a88-45a2-b017-dbca6b681a5a</t>
-  </si>
-  <si>
-    <t>877735e8-2407-45da-a3dc-527c19890f5f</t>
-  </si>
-  <si>
-    <t>61a7abc4-b9d4-4a7c-8287-1316bd955f07</t>
-  </si>
-  <si>
-    <t>0ecb761b-0d34-440c-8eee-8d9da3c4a923</t>
-  </si>
-  <si>
-    <t>88ce8b93-cad3-422c-b7f5-df423d83b939</t>
-  </si>
-  <si>
-    <t>8fc74982-3a71-4982-9cb5-af4b9017bd91</t>
-  </si>
-  <si>
-    <t>077adec4-8c75-4682-9168-6d3123921f91</t>
-  </si>
-  <si>
-    <t>9d582f70-b6ef-43e1-84f5-0f3c89933604</t>
-  </si>
-  <si>
-    <t>54ad7c88-dece-4a6b-9423-d1e45b87c01a</t>
-  </si>
-  <si>
-    <t>b06bd5d7-f6bd-4b6a-a73f-6a2afc623ae3</t>
-  </si>
-  <si>
-    <t>8a2b27c8-8587-45d2-bd83-92869b8d9cdd</t>
-  </si>
-  <si>
-    <t>da12c9fc-b68b-47fe-928b-8b01e2a9fea1</t>
-  </si>
-  <si>
-    <t>fbf29566-fd64-48d1-bf75-4dc4fce36120</t>
-  </si>
-  <si>
-    <t>62817df8-3580-45a2-8462-af545d87e573</t>
-  </si>
-  <si>
-    <t>79555e3a-e711-4720-8345-d99a3b126e2a</t>
-  </si>
-  <si>
-    <t>c13aa51c-02f4-435b-9180-d9d8a22d1161</t>
-  </si>
-  <si>
-    <t>e87e5057-3875-4a21-acfd-2c993173809b</t>
-  </si>
-  <si>
-    <t>ac3c581a-17ff-4162-bad2-cd2db03445c4</t>
+    <t>2cdc6bf2-2cac-4dfc-a607-c0e36dc6f802</t>
+  </si>
+  <si>
+    <t>7e6e067f-851c-4b2d-9725-09c905f16b98</t>
+  </si>
+  <si>
+    <t>4f32afd1-7b0f-4ba3-af85-22d3b867efc3</t>
+  </si>
+  <si>
+    <t>038a73bc-4d1a-48fb-ba82-da888430ccb3</t>
+  </si>
+  <si>
+    <t>74b05501-2d94-42f6-a503-ccd66b4d78dd</t>
+  </si>
+  <si>
+    <t>71418a54-c721-4409-9c45-bba53ec26561</t>
+  </si>
+  <si>
+    <t>4ac16c24-52b4-4060-b78f-d68b9b0e1b2d</t>
+  </si>
+  <si>
+    <t>cf78f1d9-f51d-4e4a-b24e-605e972b727f</t>
+  </si>
+  <si>
+    <t>de0a10a2-d79f-4387-98f1-7cc05ab48808</t>
+  </si>
+  <si>
+    <t>45748d1c-980d-4270-a36d-b97789e4bca6</t>
+  </si>
+  <si>
+    <t>a6d7b290-fcf5-458d-81c7-3fdbdfe5f70a</t>
+  </si>
+  <si>
+    <t>03041df1-71c0-4a3b-8d73-17c1c7284906</t>
+  </si>
+  <si>
+    <t>385a3a79-a6ea-433d-8cd5-c97a2795821c</t>
+  </si>
+  <si>
+    <t>5ee1b3f5-1b74-434e-9ea6-714998e14fb9</t>
+  </si>
+  <si>
+    <t>fa3c51b0-16b2-4c8b-a212-d01f9c1709a7</t>
+  </si>
+  <si>
+    <t>67659c40-ee76-4660-b744-b494e4e6162b</t>
+  </si>
+  <si>
+    <t>7c42b726-25e1-405c-975d-8720dc3a2a6a</t>
+  </si>
+  <si>
+    <t>b2abd50e-5820-4f09-a56d-df0db8c03450</t>
+  </si>
+  <si>
+    <t>1ecfe948-1d6c-430e-be26-18774134ebf2</t>
+  </si>
+  <si>
+    <t>8a071566-5bd2-4557-9c52-9e36992b9c5a</t>
   </si>
   <si>
     <t>Mode</t>

</xml_diff>

<commit_message>
Fix template generation enum TypeError
</commit_message>
<xml_diff>
--- a/experiments/xls/measurements_input.xlsx
+++ b/experiments/xls/measurements_input.xlsx
@@ -1,33 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ak27/programming/cellgeni/imaging_tracking/experiments/xls/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124B323A-EB57-8747-8813-F4B4FF0FBDAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="33480" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>UUID</t>
   </si>
   <si>
+    <t>297892a3-43d8-404d-9389-183b11b583dd</t>
+  </si>
+  <si>
+    <t>99c7bb6e-5241-4c87-9010-57126604a958</t>
+  </si>
+  <si>
+    <t>f83ee2e5-c156-42c2-9bbb-a11759213015</t>
+  </si>
+  <si>
+    <t>9ce498ac-e4b2-4eec-86c9-fa23ceb2a12f</t>
+  </si>
+  <si>
+    <t>7ab89b0f-cc19-428e-9634-beefe033f2be</t>
+  </si>
+  <si>
+    <t>5bb67546-1e36-45e4-a72f-70375d0ae7ed</t>
+  </si>
+  <si>
+    <t>4e5af812-aa05-4eb9-8a16-18a17bd00416</t>
+  </si>
+  <si>
+    <t>8034df41-cffe-481a-bc75-ac032079143b</t>
+  </si>
+  <si>
+    <t>4ccdb87f-87e5-479b-99de-5606cafdc2ca</t>
+  </si>
+  <si>
+    <t>15a7c676-35e3-420d-858d-955e524d8767</t>
+  </si>
+  <si>
+    <t>033c2234-7027-4113-8012-5cab4b7a3ffa</t>
+  </si>
+  <si>
+    <t>77a1d51c-fd39-4d65-b44d-d00801fb56a3</t>
+  </si>
+  <si>
+    <t>b7beba59-506d-4f5a-9465-ec8a8badd158</t>
+  </si>
+  <si>
+    <t>6194dc53-0b70-4e7f-8c79-eede8e98d9d3</t>
+  </si>
+  <si>
+    <t>df143cc1-7b69-4b0d-b8cb-b5525c7884cf</t>
+  </si>
+  <si>
+    <t>e898ab0c-c377-4dde-a303-db233f037b24</t>
+  </si>
+  <si>
+    <t>c5eae15d-b120-4b11-b148-7d1a45803212</t>
+  </si>
+  <si>
+    <t>719e5546-fa09-4b3d-ac9b-43bf082c9ee9</t>
+  </si>
+  <si>
+    <t>8f6bf762-f1ca-4261-8c21-492f2ca8adb8</t>
+  </si>
+  <si>
+    <t>1a787f50-9a8f-4aeb-bee5-97e2d579cc53</t>
+  </si>
+  <si>
     <t>Mode</t>
   </si>
   <si>
+    <t>Ignore</t>
+  </si>
+  <si>
     <t>Researcher</t>
   </si>
   <si>
@@ -43,13 +100,13 @@
     <t>Automated_SlideN</t>
   </si>
   <si>
-    <t>Slide barcode id</t>
+    <t>Slide</t>
   </si>
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Image cycle</t>
+    <t>Image_cycle</t>
   </si>
   <si>
     <t>Channel-Target1</t>
@@ -103,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,14 +207,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -204,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,27 +285,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,24 +319,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,123 +494,303 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="26" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" customWidth="1"/>
+    <col min="23" max="23" width="20.7109375" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" customWidth="1"/>
+    <col min="25" max="25" width="20.7109375" customWidth="1"/>
+    <col min="26" max="26" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
+      <c r="B21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mode" prompt="Choose mode" sqref="B2:B101" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Ignore,Create or update,Delete"</formula1>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Mode" prompt="Choose mode" sqref="B2:B101">
+      <formula1>"Create or update,Ignore,Delete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Researcher" prompt="Choose researcher" sqref="C2:C101" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"A_K,M_W,KR"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Researcher" prompt="Choose researcher" sqref="C2:C101">
+      <formula1>"KR,ET"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Project" prompt="Choose project" sqref="D2:D101" xr:uid="{00000000-0002-0000-0000-000002000000}">
-      <formula1>"ML_HEA,KB_CAH,TM_RCC"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Project" prompt="Choose project" sqref="D2:D101">
+      <formula1>"HZ_HLB,RV_END"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G101" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G101">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Technology" prompt="Choose technology" sqref="I2:I101" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>"RNAscope 4-plex,RNAscope 8-plex,RNAscope 3-plex + IHC"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Technology" prompt="Choose technology" sqref="I2:I101">
+      <formula1>"RNAscope HiPlex,RNAscope 3-plex + IHC"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J101" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J101">
       <formula1>10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Channel-target pair" prompt="Choose channel-target pair" sqref="K2:O101" xr:uid="{00000000-0002-0000-0000-000006000000}">
-      <formula1>"Atto 425 -&gt; MYH11,Atto 425 -&gt; dapB,Atto 425 -&gt; POLR2A,Opal 520 -&gt; MYH11,Opal 520 -&gt; dapB,Opal 520 -&gt; POLR2A,DAPI -&gt; Nucleus,Opal 520 -&gt; PECAM1 (IHC),Opal 570 -&gt; CA9,Opal 650 -&gt; TPSB2,Atto 425 -&gt; CD68,Opal 570 -&gt; CMET"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Team directory" prompt="Choose team directory" sqref="Z2:Z101" xr:uid="{00000000-0002-0000-0000-00000B000000}">
-      <formula1>"t283_imaging,t876_imaging"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Team directory" prompt="Choose team directory" sqref="Z2:Z101">
+      <formula1>""</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>